<commit_message>
Minor UI tweaks and package updates
</commit_message>
<xml_diff>
--- a/Documentation/IssueTrackerSchedule.xlsx
+++ b/Documentation/IssueTrackerSchedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\IssueTrackerProject\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\IssueTracker\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC6379B-FEBF-4736-AD47-8B5B2E569361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39884F03-3EAF-435A-8731-E4840750F3BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1D283BD5-9558-40FA-A3D8-8D5CF7D073E2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
   <si>
     <t>Bug Tracker Schedule</t>
   </si>
@@ -211,6 +212,81 @@
   </si>
   <si>
     <t>Refresh javascript knowledge</t>
+  </si>
+  <si>
+    <t>started at 1:40</t>
+  </si>
+  <si>
+    <t>make page layouts</t>
+  </si>
+  <si>
+    <t>started 11:32</t>
+  </si>
+  <si>
+    <t>started 8:35pm</t>
+  </si>
+  <si>
+    <t>started 11:37</t>
+  </si>
+  <si>
+    <t>started 12:49</t>
+  </si>
+  <si>
+    <t>check to see if you need to add .vs and packages folder to git ignore</t>
+  </si>
+  <si>
+    <t>setup base website</t>
+  </si>
+  <si>
+    <t>get place holder icons</t>
+  </si>
+  <si>
+    <t>Refresh Javascript knowledge</t>
+  </si>
+  <si>
+    <t>Learn how to add graphic box objects to website</t>
+  </si>
+  <si>
+    <t>Learn how to add functionality to buttons</t>
+  </si>
+  <si>
+    <t>watch asp.net database vid</t>
+  </si>
+  <si>
+    <t>how to generate new list items in html</t>
+  </si>
+  <si>
+    <t>where to add css for customization</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>1. Directly in your view file(.cshtml/.aspx).</t>
+  </si>
+  <si>
+    <t>2. Separate css files inside Content/css folder</t>
+  </si>
+  <si>
+    <t>get rid of tester.css</t>
+  </si>
+  <si>
+    <t>adjust Site.css</t>
+  </si>
+  <si>
+    <t>started 2:54</t>
+  </si>
+  <si>
+    <t>started 11:57</t>
+  </si>
+  <si>
+    <t>never really started</t>
+  </si>
+  <si>
+    <t>setup site how I want</t>
+  </si>
+  <si>
+    <t>watch database tutorial</t>
   </si>
 </sst>
 </file>
@@ -220,7 +296,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +310,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -262,11 +344,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -584,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35E8C7C-71FA-4C65-822A-559C850A9297}">
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,6 +824,15 @@
       <c r="L3" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="S3" t="s">
+        <v>78</v>
+      </c>
+      <c r="T3" t="s">
+        <v>78</v>
+      </c>
+      <c r="V3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -759,8 +854,32 @@
       <c r="H4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -773,6 +892,33 @@
       <c r="L5" t="s">
         <v>55</v>
       </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" t="s">
+        <v>67</v>
+      </c>
+      <c r="T5" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -781,6 +927,30 @@
       <c r="L6" t="s">
         <v>56</v>
       </c>
+      <c r="M6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" t="s">
+        <v>61</v>
+      </c>
+      <c r="S6" t="s">
+        <v>61</v>
+      </c>
+      <c r="T6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -789,6 +959,24 @@
       <c r="L7" t="s">
         <v>57</v>
       </c>
+      <c r="M7" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" t="s">
+        <v>57</v>
+      </c>
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -797,6 +985,30 @@
       <c r="L8" t="s">
         <v>58</v>
       </c>
+      <c r="M8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R8" t="s">
+        <v>66</v>
+      </c>
+      <c r="S8" t="s">
+        <v>66</v>
+      </c>
+      <c r="T8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -805,6 +1017,21 @@
       <c r="L9" t="s">
         <v>59</v>
       </c>
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -844,6 +1071,33 @@
       <c r="L12" t="s">
         <v>53</v>
       </c>
+      <c r="M12" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="4">
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="O12" t="s">
+        <v>62</v>
+      </c>
+      <c r="P12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>64</v>
+      </c>
+      <c r="R12" t="s">
+        <v>65</v>
+      </c>
+      <c r="S12" t="s">
+        <v>80</v>
+      </c>
+      <c r="T12" t="s">
+        <v>81</v>
+      </c>
+      <c r="U12" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
@@ -875,17 +1129,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -899,8 +1153,16 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -909,67 +1171,107 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E23" s="2"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R23" s="2"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="33" x14ac:dyDescent="0.25">
+      <c r="R33" t="s">
+        <v>74</v>
+      </c>
+      <c r="S33" t="s">
+        <v>75</v>
+      </c>
+      <c r="T33" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="33" x14ac:dyDescent="0.25">
+      <c r="T34" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>